<commit_message>
created new tests to replace the ones associated with functions that were deleted when old (annual) couplePV calc deleted
</commit_message>
<xml_diff>
--- a/Notes on SS Rules/retroactive application logic plan.xlsx
+++ b/Notes on SS Rules/retroactive application logic plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalindap/Dropbox/SimpleSubjects/OpenSSaccompanyingStuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalindap/Dropbox/SimpleSubjects/open-social-security/Notes on SS Rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02AE12D-9C6F-4B4A-832D-BF92DC481F6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9756B93-550C-4147-9826-68D97731BCF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="460" windowWidth="39540" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Single</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>This means that when retroactive application happens, it will show an additional row (for prior year) in some cases. But that's OK and not misleading, because only time it's actually an *additional* row is when there are no benefits in that prior year without the retroactive application. If there are some benefits in that prior year without retroactive app, it will be included in table regardless of whether retroactive app happens or not. Concern had been scenario in which one person is getting benefit in prior year regardless of whether other person files retroactive app or not -- but then the row only appears in case of retroactive app (thereby possibly making retroactive app look like it has larger effect than it does). This solution handles that concern though, because in this case the prior year gets a row either way.</t>
+  </si>
+  <si>
+    <t>https://secure.ssa.gov/poms.nsf/lnx/0200204030</t>
   </si>
 </sst>
 </file>
@@ -163,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -195,16 +198,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -524,7 +530,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,6 +548,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>0</v>
@@ -554,7 +565,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="153" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -568,14 +579,14 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -583,13 +594,13 @@
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -597,18 +608,18 @@
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="203" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">

</xml_diff>